<commit_message>
regular update, will be changed.
</commit_message>
<xml_diff>
--- a/mega2560_pins/管脚对应.xlsx
+++ b/mega2560_pins/管脚对应.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>SLC</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -33,10 +33,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>TX0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -45,22 +41,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>5V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>VIN</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GND</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>5V</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>3.3V</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -133,7 +117,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>GND</t>
+    <t>GND1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GND4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5V1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5V2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5V3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>5V4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -157,7 +169,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -167,6 +179,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,7 +212,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -480,7 +498,7 @@
   <dimension ref="A1:AR40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AJ21" sqref="AJ21"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -614,8 +632,8 @@
       <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
+      <c r="E2" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="F2" s="2">
         <v>13</v>
@@ -722,10 +740,10 @@
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>5</v>
       </c>
       <c r="V3" s="2"/>
       <c r="W3" s="2"/>
@@ -741,9 +759,11 @@
       <c r="AG3" s="2"/>
       <c r="AH3" s="2"/>
       <c r="AI3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="AJ3" s="4"/>
+        <v>28</v>
+      </c>
+      <c r="AJ3" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="AK3" s="2"/>
       <c r="AL3" s="2"/>
       <c r="AM3" s="2"/>
@@ -1605,8 +1625,8 @@
       <c r="AG20" s="2"/>
       <c r="AH20" s="2"/>
       <c r="AI20" s="2"/>
-      <c r="AJ20" s="2" t="s">
-        <v>28</v>
+      <c r="AJ20" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="AK20" s="2"/>
       <c r="AL20" s="2"/>
@@ -1670,78 +1690,78 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F22" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>8</v>
+      <c r="H22" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L22" s="3"/>
       <c r="M22" s="3"/>
       <c r="N22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O22" s="2" t="s">
+      <c r="S22" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P22" s="2" t="s">
+      <c r="T22" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q22" s="2" t="s">
+      <c r="U22" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="U22" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AA22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AB22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Y22" s="2" t="s">
+      <c r="AC22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Z22" s="2" t="s">
+      <c r="AD22" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AA22" s="2" t="s">
+      <c r="AE22" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="AB22" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="AC22" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AD22" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AE22" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
@@ -2580,9 +2600,6 @@
       <c r="AR40" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="AI3:AJ3"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>